<commit_message>
add players on spreadsheat
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myoffice.accenture.com/personal/ligia_v_nogueira_accenture_com/Documents/Documents/MeuGit/ProjetoPelada/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{BFFFCAF0-1EE4-4338-B981-AE87E6791D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA68C36A-48D8-463C-8BEA-D3F9D405A323}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="8_{BFFFCAF0-1EE4-4338-B981-AE87E6791D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{999A871B-2231-4208-BBA3-6A863980937E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{EB057D50-8FB1-4376-9EFE-61206BA62CE4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
   <si>
     <t>Ligia</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>Meio-Campo</t>
+  </si>
+  <si>
+    <t>Helen</t>
+  </si>
+  <si>
+    <t>Isadora</t>
   </si>
 </sst>
 </file>
@@ -179,9 +185,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -219,7 +225,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -325,7 +331,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -467,7 +473,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -475,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B2A35C9-574C-4D2C-A806-9A40CCBE067F}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -647,7 +653,7 @@
         <v>20</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C15" s="1">
         <v>5</v>
@@ -695,6 +701,28 @@
       </c>
       <c r="C19" s="1">
         <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjustments to the name and position columns.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myoffice.accenture.com/personal/ligia_v_nogueira_accenture_com/Documents/Documents/MeuGit/ProjetoPelada/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{BFFFCAF0-1EE4-4338-B981-AE87E6791D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{999A871B-2231-4208-BBA3-6A863980937E}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{BFFFCAF0-1EE4-4338-B981-AE87E6791D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90F0B231-F076-447A-A842-D1D26B3181B9}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{EB057D50-8FB1-4376-9EFE-61206BA62CE4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{EB057D50-8FB1-4376-9EFE-61206BA62CE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -89,12 +89,6 @@
     <t>Camila</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>position</t>
-  </si>
-  <si>
     <t>points</t>
   </si>
   <si>
@@ -114,6 +108,12 @@
   </si>
   <si>
     <t>Isadora</t>
+  </si>
+  <si>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>Posição</t>
   </si>
 </sst>
 </file>
@@ -484,7 +484,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -496,13 +496,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -510,7 +510,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1">
         <v>5</v>
@@ -521,7 +521,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1">
         <v>5</v>
@@ -532,7 +532,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1">
         <v>4</v>
@@ -543,7 +543,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
@@ -554,7 +554,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
@@ -565,7 +565,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -576,7 +576,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1">
         <v>3</v>
@@ -587,7 +587,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1">
         <v>4</v>
@@ -598,7 +598,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C10" s="1">
         <v>4</v>
@@ -609,7 +609,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11" s="1">
         <v>5</v>
@@ -620,7 +620,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C12" s="1">
         <v>4</v>
@@ -631,7 +631,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
@@ -642,7 +642,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C14" s="1">
         <v>2</v>
@@ -650,10 +650,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C15" s="1">
         <v>5</v>
@@ -664,7 +664,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C16" s="1">
         <v>3</v>
@@ -675,7 +675,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C17" s="1">
         <v>5</v>
@@ -686,7 +686,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C18" s="1">
         <v>5</v>
@@ -697,7 +697,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C19" s="1">
         <v>2</v>
@@ -705,10 +705,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
@@ -716,10 +716,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C21" s="1">
         <v>1</v>

</xml_diff>